<commit_message>
Changes related to register and login locators
</commit_message>
<xml_diff>
--- a/src/main/resources/input_data.xlsx
+++ b/src/main/resources/input_data.xlsx
@@ -62,32 +62,10 @@
     <t xml:space="preserve">https://console.uat.asians.group/#/domain/list</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Confirm</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Password</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Please specify username.
-Please specify email.
-Please specify password.</t>
+    <t xml:space="preserve">ConfirmPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please specify username.Please specify email.Please specify password.</t>
   </si>
   <si>
     <t xml:space="preserve">sndp741s06@gmail.com</t>
@@ -112,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -139,20 +117,6 @@
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF111111"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -219,12 +183,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -288,7 +252,7 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF111111"/>
+      <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
@@ -335,12 +299,12 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -424,7 +388,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -456,7 +420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="38.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Revert "Changes related to register and login locators"
This reverts commit c725107449b23a677bec83623c427c6a37c265fc.
</commit_message>
<xml_diff>
--- a/src/main/resources/input_data.xlsx
+++ b/src/main/resources/input_data.xlsx
@@ -62,10 +62,32 @@
     <t xml:space="preserve">https://console.uat.asians.group/#/domain/list</t>
   </si>
   <si>
-    <t xml:space="preserve">ConfirmPassword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please specify username.Please specify email.Please specify password.</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Confirm</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Password</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Please specify username.
+Please specify email.
+Please specify password.</t>
   </si>
   <si>
     <t xml:space="preserve">sndp741s06@gmail.com</t>
@@ -90,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -117,6 +139,20 @@
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF111111"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -183,12 +219,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -252,7 +288,7 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF111111"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
@@ -299,12 +335,12 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -388,7 +424,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -420,7 +456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="38.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added updated locators for login and register classes.
</commit_message>
<xml_diff>
--- a/src/main/resources/input_data.xlsx
+++ b/src/main/resources/input_data.xlsx
@@ -62,32 +62,10 @@
     <t xml:space="preserve">https://console.uat.asians.group/#/domain/list</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Confirm</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Password</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Please specify username.
-Please specify email.
-Please specify password.</t>
+    <t xml:space="preserve">ConfirmPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please specify username.Please specify email.Please specify password.</t>
   </si>
   <si>
     <t xml:space="preserve">sndp741s06@gmail.com</t>
@@ -112,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -139,20 +117,6 @@
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF111111"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -219,12 +183,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -288,7 +252,7 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF111111"/>
+      <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
@@ -335,12 +299,12 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -424,7 +388,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -456,7 +420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="38.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>